<commit_message>
Update Allograft Rejection Spreadsheet.xlsx
</commit_message>
<xml_diff>
--- a/data/Allograft Rejection Spreadsheet.xlsx
+++ b/data/Allograft Rejection Spreadsheet.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harryrobertson/Desktop/PhD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unisydneyedu-my.sharepoint.com/personal/qigu9636_uni_sydney_edu_au/Documents/Unit of Study/2022 Semester 1/DATA3888/Data3888-KidneyA1/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{149E7D62-D5E6-DF43-8E20-F7D37F76A7A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{149E7D62-D5E6-DF43-8E20-F7D37F76A7A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7BED7BB-77EB-42D3-8F4F-927D317B8D3A}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16180" xr2:uid="{078EEEE2-A789-D948-B4CF-13AB17F578B0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{078EEEE2-A789-D948-B4CF-13AB17F578B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$59</definedName>
+  </definedNames>
   <calcPr calcId="181029" iterateCount="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -23,9 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="267">
   <si>
     <t>Database</t>
   </si>
@@ -820,6 +821,21 @@
   </si>
   <si>
     <t>Molecular mapping of interstitial lung disease reveals a phenotypically distinct senescent basal epithelial cell population.</t>
+  </si>
+  <si>
+    <t>Hangyi Wu</t>
+  </si>
+  <si>
+    <t>Qinlin Gu</t>
+  </si>
+  <si>
+    <t>Xuening Ni</t>
+  </si>
+  <si>
+    <t>Danying Sun</t>
+  </si>
+  <si>
+    <t>Yuye Zhou</t>
   </si>
 </sst>
 </file>
@@ -953,8 +969,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -970,7 +986,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1266,31 +1282,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D030C5-8C54-2A48-90BC-6F06473898BD}">
-  <dimension ref="A1:O59"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:P59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.5" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" style="13" customWidth="1"/>
-    <col min="9" max="9" width="19.1640625" style="13" customWidth="1"/>
-    <col min="11" max="11" width="14.83203125" customWidth="1"/>
-    <col min="12" max="12" width="18.83203125" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" customWidth="1"/>
-    <col min="14" max="14" width="187.5" customWidth="1"/>
-    <col min="15" max="15" width="35.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.09765625" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="148.796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1300,44 +1319,44 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1347,38 +1366,41 @@
       <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
       <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
         <v>63</v>
       </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>2019</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>95</v>
       </c>
-      <c r="M2" s="4">
+      <c r="N2" s="4">
         <v>31378695</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1388,41 +1410,44 @@
       <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
       <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
         <v>63</v>
       </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="J3" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>2012</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>56</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>139</v>
       </c>
-      <c r="M3" s="4">
+      <c r="N3" s="4">
         <v>22335458</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1432,38 +1457,41 @@
       <c r="C4" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" t="s">
+        <v>263</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
       <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
         <v>63</v>
       </c>
-      <c r="G4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="J4" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>2019</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>117</v>
       </c>
-      <c r="M4" s="4">
+      <c r="N4" s="4">
         <v>31378695</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1473,41 +1501,44 @@
       <c r="C5" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" t="s">
+        <v>263</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
       <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
         <v>63</v>
       </c>
-      <c r="G5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="J5" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>2015</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>18</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>209</v>
       </c>
-      <c r="M5" s="4">
+      <c r="N5" s="4">
         <v>25925804</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1517,41 +1548,41 @@
       <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
       <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
         <v>24</v>
       </c>
-      <c r="G6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="J6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>2016</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>39</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>27</v>
       </c>
-      <c r="M6" s="4">
+      <c r="N6" s="4">
         <v>27898719</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1561,38 +1592,38 @@
       <c r="C7" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
       <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
         <v>24</v>
       </c>
-      <c r="G7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="J7" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>2006</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>285</v>
       </c>
-      <c r="M7" s="4">
+      <c r="N7" s="4">
         <v>16433769</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="O7" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1602,38 +1633,41 @@
       <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E8" t="s">
-        <v>17</v>
-      </c>
       <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
         <v>24</v>
       </c>
-      <c r="G8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="J8" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>2003</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>67</v>
       </c>
-      <c r="M8" s="4">
+      <c r="N8" s="4">
         <v>12853585</v>
       </c>
-      <c r="N8" s="9" t="s">
+      <c r="O8" s="9" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1643,41 +1677,44 @@
       <c r="C9" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" t="s">
+        <v>263</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
       <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
         <v>24</v>
       </c>
-      <c r="G9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="J9" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>2014</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>109</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>191</v>
       </c>
-      <c r="M9" s="4">
+      <c r="N9" s="4">
         <v>24725967</v>
       </c>
-      <c r="N9" s="2" t="s">
+      <c r="O9" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1687,41 +1724,44 @@
       <c r="C10" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" t="s">
+        <v>263</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
       <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" t="s">
         <v>24</v>
       </c>
-      <c r="G10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="J10" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>2014</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>40</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>204</v>
       </c>
-      <c r="M10" s="4">
+      <c r="N10" s="4">
         <v>25387159</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="O10" s="5" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1731,41 +1771,41 @@
       <c r="C11" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="E11" t="s">
-        <v>17</v>
-      </c>
       <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s">
         <v>24</v>
       </c>
-      <c r="G11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="J11" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>2009</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>22</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>227</v>
       </c>
-      <c r="M11" s="4">
+      <c r="N11" s="4">
         <v>19938108</v>
       </c>
-      <c r="N11" s="2" t="s">
+      <c r="O11" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1775,41 +1815,41 @@
       <c r="C12" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="E12" t="s">
-        <v>17</v>
-      </c>
       <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
         <v>24</v>
       </c>
-      <c r="G12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="J12" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>2016</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>74</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>237</v>
       </c>
-      <c r="M12" s="4">
+      <c r="N12" s="4">
         <v>26517400</v>
       </c>
-      <c r="N12" s="2" t="s">
+      <c r="O12" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1819,41 +1859,44 @@
       <c r="C13" t="s">
         <v>170</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" t="s">
+        <v>263</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E13" t="s">
-        <v>17</v>
-      </c>
       <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="s">
         <v>171</v>
       </c>
-      <c r="G13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="J13" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>2013</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>115</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>174</v>
       </c>
-      <c r="M13" s="4">
+      <c r="N13" s="4">
         <v>26484130</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="O13" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1863,41 +1906,44 @@
       <c r="C14" t="s">
         <v>170</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" t="s">
+        <v>264</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E14" t="s">
-        <v>17</v>
-      </c>
       <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" t="s">
         <v>171</v>
       </c>
-      <c r="G14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="J14" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>2014</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>55</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>40</v>
       </c>
-      <c r="M14" s="4">
+      <c r="N14" s="4">
         <v>24698514</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="O14" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1907,41 +1953,41 @@
       <c r="C15" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E15" t="s">
-        <v>17</v>
-      </c>
       <c r="F15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" t="s">
         <v>18</v>
       </c>
-      <c r="G15" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="13" t="s">
+      <c r="H15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="I15" s="13" t="s">
+      <c r="J15" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>2005</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>63</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>32</v>
       </c>
-      <c r="M15" s="4">
+      <c r="N15" s="4">
         <v>16794196</v>
       </c>
-      <c r="N15" s="2" t="s">
+      <c r="O15" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1951,41 +1997,41 @@
       <c r="C16" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E16" t="s">
-        <v>17</v>
-      </c>
       <c r="F16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" t="s">
         <v>18</v>
       </c>
-      <c r="G16" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" s="13" t="s">
+      <c r="H16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="J16" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>2006</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>9</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>20</v>
       </c>
-      <c r="M16" s="4">
+      <c r="N16" s="4">
         <v>16780603</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1995,41 +2041,41 @@
       <c r="C17" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E17" t="s">
-        <v>17</v>
-      </c>
       <c r="F17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" t="s">
         <v>18</v>
       </c>
-      <c r="G17" t="s">
-        <v>19</v>
-      </c>
-      <c r="H17" s="13" t="s">
+      <c r="H17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="J17" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>2006</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>25</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>40</v>
       </c>
-      <c r="M17" s="4">
+      <c r="N17" s="4">
         <v>16794196</v>
       </c>
-      <c r="N17" s="2" t="s">
+      <c r="O17" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -2039,41 +2085,41 @@
       <c r="C18" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E18" t="s">
-        <v>17</v>
-      </c>
       <c r="F18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" t="s">
         <v>18</v>
       </c>
-      <c r="G18" t="s">
-        <v>19</v>
-      </c>
-      <c r="H18" s="13" t="s">
+      <c r="H18" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="I18" s="13" t="s">
+      <c r="J18" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>2008</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>26</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>44</v>
       </c>
-      <c r="M18" s="4">
+      <c r="N18" s="4">
         <v>21555702</v>
       </c>
-      <c r="N18" s="2" t="s">
+      <c r="O18" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2083,32 +2129,35 @@
       <c r="C19" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" t="s">
+        <v>264</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E19" t="s">
-        <v>17</v>
-      </c>
       <c r="F19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" t="s">
         <v>18</v>
       </c>
-      <c r="G19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19" s="13" t="s">
+      <c r="H19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="I19" s="14" t="s">
+      <c r="J19" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>2019</v>
       </c>
-      <c r="O19" s="8" t="s">
+      <c r="P19" s="8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -2118,41 +2167,44 @@
       <c r="C20" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" t="s">
+        <v>264</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E20" t="s">
-        <v>17</v>
-      </c>
       <c r="F20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" t="s">
         <v>18</v>
       </c>
-      <c r="G20" t="s">
-        <v>19</v>
-      </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="I20" s="13" t="s">
+      <c r="J20" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>2010</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>36</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>73</v>
       </c>
-      <c r="M20" s="4">
+      <c r="N20" s="4">
         <v>20150539</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -2162,35 +2214,38 @@
       <c r="C21" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" t="s">
+        <v>264</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E21" t="s">
-        <v>17</v>
-      </c>
       <c r="F21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" t="s">
         <v>18</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>76</v>
       </c>
-      <c r="H21" s="13" t="s">
+      <c r="I21" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="I21" s="13" t="s">
+      <c r="J21" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>2020</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>7</v>
       </c>
-      <c r="M21" s="4">
+      <c r="N21" s="4">
         <v>32669324</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -2200,38 +2255,41 @@
       <c r="C22" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" t="s">
+        <v>264</v>
+      </c>
+      <c r="E22" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E22" t="s">
-        <v>17</v>
-      </c>
       <c r="F22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" t="s">
         <v>18</v>
       </c>
-      <c r="G22" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" s="13" t="s">
+      <c r="H22" t="s">
+        <v>19</v>
+      </c>
+      <c r="I22" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="I22" s="13" t="s">
+      <c r="J22" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>2004</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>31</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>82</v>
       </c>
-      <c r="M22" s="4">
+      <c r="N22" s="4">
         <v>15307835</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -2241,41 +2299,44 @@
       <c r="C23" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" t="s">
+        <v>264</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E23" t="s">
-        <v>17</v>
-      </c>
       <c r="F23" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" t="s">
         <v>18</v>
       </c>
-      <c r="G23" t="s">
-        <v>19</v>
-      </c>
-      <c r="H23" s="13" t="s">
+      <c r="H23" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="I23" s="13" t="s">
+      <c r="J23" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>2009</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>119</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>86</v>
       </c>
-      <c r="M23" s="4">
+      <c r="N23" s="4">
         <v>21130165</v>
       </c>
-      <c r="N23" s="2" t="s">
+      <c r="O23" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -2285,35 +2346,38 @@
       <c r="C24" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" t="s">
+        <v>264</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E24" t="s">
-        <v>17</v>
-      </c>
       <c r="F24" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" t="s">
         <v>18</v>
       </c>
-      <c r="G24" t="s">
-        <v>19</v>
-      </c>
-      <c r="H24" s="13" t="s">
+      <c r="H24" t="s">
+        <v>19</v>
+      </c>
+      <c r="I24" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="I24" s="13" t="s">
+      <c r="J24" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>2011</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <v>113</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -2323,44 +2387,47 @@
       <c r="C25" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" t="s">
+        <v>264</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E25" t="s">
-        <v>17</v>
-      </c>
       <c r="F25" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" t="s">
         <v>18</v>
       </c>
-      <c r="G25" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="13" t="s">
+      <c r="H25" t="s">
+        <v>19</v>
+      </c>
+      <c r="I25" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="I25" s="13" t="s">
+      <c r="J25" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>2014</v>
       </c>
-      <c r="K25">
+      <c r="L25">
         <v>66</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>99</v>
       </c>
-      <c r="M25" s="4">
+      <c r="N25" s="4">
         <v>23437201</v>
       </c>
-      <c r="N25" s="2" t="s">
+      <c r="O25" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="O25" t="s">
+      <c r="P25" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -2370,41 +2437,44 @@
       <c r="C26" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" t="s">
+        <v>262</v>
+      </c>
+      <c r="E26" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E26" t="s">
-        <v>17</v>
-      </c>
       <c r="F26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" t="s">
         <v>18</v>
       </c>
-      <c r="G26" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="13" t="s">
+      <c r="H26" t="s">
+        <v>19</v>
+      </c>
+      <c r="I26" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="I26" s="13" t="s">
+      <c r="J26" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>2017</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <v>79</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>86</v>
       </c>
-      <c r="M26" s="4">
+      <c r="N26" s="4">
         <v>27165815</v>
       </c>
-      <c r="N26" s="2" t="s">
+      <c r="O26" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -2414,38 +2484,41 @@
       <c r="C27" t="s">
         <v>16</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" t="s">
+        <v>262</v>
+      </c>
+      <c r="E27" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E27" t="s">
-        <v>17</v>
-      </c>
       <c r="F27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" t="s">
         <v>18</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>76</v>
       </c>
-      <c r="H27" s="13" t="s">
+      <c r="I27" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="I27" s="13" t="s">
+      <c r="J27" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>2018</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <v>7</v>
       </c>
-      <c r="M27" s="4">
+      <c r="N27" s="4">
         <v>29980650</v>
       </c>
-      <c r="N27" s="2" t="s">
+      <c r="O27" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -2455,41 +2528,44 @@
       <c r="C28" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" t="s">
+        <v>262</v>
+      </c>
+      <c r="E28" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E28" t="s">
-        <v>17</v>
-      </c>
       <c r="F28" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" t="s">
         <v>18</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>151</v>
       </c>
-      <c r="H28" s="13" t="s">
+      <c r="I28" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="I28" s="13" t="s">
+      <c r="J28" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>2019</v>
       </c>
-      <c r="K28">
+      <c r="L28">
         <v>235</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>182</v>
       </c>
-      <c r="M28" s="4">
+      <c r="N28" s="4">
         <v>31167967</v>
       </c>
-      <c r="N28" s="2" t="s">
+      <c r="O28" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -2499,35 +2575,38 @@
       <c r="C29" t="s">
         <v>47</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" t="s">
+        <v>262</v>
+      </c>
+      <c r="E29" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E29" t="s">
-        <v>17</v>
-      </c>
       <c r="F29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" t="s">
         <v>18</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>188</v>
       </c>
-      <c r="H29" s="13" t="s">
+      <c r="I29" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="I29" s="13" t="s">
+      <c r="J29" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>2020</v>
       </c>
-      <c r="K29">
+      <c r="L29">
         <v>10</v>
       </c>
-      <c r="M29" s="4">
+      <c r="N29" s="4">
         <v>32669324</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -2537,38 +2616,41 @@
       <c r="C30" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" t="s">
+        <v>262</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E30" t="s">
-        <v>17</v>
-      </c>
       <c r="F30" t="s">
+        <v>17</v>
+      </c>
+      <c r="G30" t="s">
         <v>18</v>
       </c>
-      <c r="G30" t="s">
-        <v>19</v>
-      </c>
-      <c r="H30" s="13" t="s">
+      <c r="H30" t="s">
+        <v>19</v>
+      </c>
+      <c r="I30" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="I30" s="13" t="s">
+      <c r="J30" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>2004</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <v>31</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>82</v>
       </c>
-      <c r="M30" s="4">
+      <c r="N30" s="4">
         <v>15307835</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -2578,41 +2660,44 @@
       <c r="C31" t="s">
         <v>47</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" t="s">
+        <v>262</v>
+      </c>
+      <c r="E31" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E31" t="s">
-        <v>17</v>
-      </c>
       <c r="F31" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" t="s">
         <v>18</v>
       </c>
-      <c r="G31" t="s">
-        <v>19</v>
-      </c>
-      <c r="H31" s="13" t="s">
+      <c r="H31" t="s">
+        <v>19</v>
+      </c>
+      <c r="I31" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="I31" s="13" t="s">
+      <c r="J31" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <v>2010</v>
       </c>
-      <c r="K31">
+      <c r="L31">
         <v>24</v>
       </c>
-      <c r="L31" t="s">
+      <c r="M31" t="s">
         <v>86</v>
       </c>
-      <c r="M31" s="4">
+      <c r="N31" s="4">
         <v>20208531</v>
       </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -2622,41 +2707,44 @@
       <c r="C32" t="s">
         <v>47</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" t="s">
+        <v>262</v>
+      </c>
+      <c r="E32" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E32" t="s">
-        <v>17</v>
-      </c>
       <c r="F32" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" t="s">
         <v>18</v>
       </c>
-      <c r="G32" t="s">
-        <v>19</v>
-      </c>
-      <c r="H32" s="13" t="s">
+      <c r="H32" t="s">
+        <v>19</v>
+      </c>
+      <c r="I32" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="I32" s="13" t="s">
+      <c r="J32" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <v>2011</v>
       </c>
-      <c r="K32">
+      <c r="L32">
         <v>24</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M32" t="s">
         <v>199</v>
       </c>
-      <c r="M32" s="4">
+      <c r="N32" s="4">
         <v>21827613</v>
       </c>
-      <c r="N32" s="2" t="s">
+      <c r="O32" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -2666,35 +2754,38 @@
       <c r="C33" t="s">
         <v>47</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" t="s">
+        <v>262</v>
+      </c>
+      <c r="E33" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E33" t="s">
-        <v>17</v>
-      </c>
       <c r="F33" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" t="s">
         <v>18</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>76</v>
       </c>
-      <c r="H33" s="13" t="s">
+      <c r="I33" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="I33" s="13" t="s">
+      <c r="J33" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <v>2021</v>
       </c>
-      <c r="K33">
+      <c r="L33">
         <v>3</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -2704,41 +2795,41 @@
       <c r="C34" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="E34" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="E34" t="s">
-        <v>17</v>
-      </c>
       <c r="F34" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" t="s">
         <v>18</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>220</v>
       </c>
-      <c r="H34" s="14" t="s">
+      <c r="I34" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="I34" s="13" t="s">
+      <c r="J34" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <v>2008</v>
       </c>
-      <c r="K34">
+      <c r="L34">
         <v>26</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
         <v>86</v>
       </c>
-      <c r="M34" s="4">
+      <c r="N34" s="4">
         <v>18639552</v>
       </c>
-      <c r="N34" s="2" t="s">
+      <c r="O34" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -2748,41 +2839,41 @@
       <c r="C35" t="s">
         <v>16</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="E35" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="E35" t="s">
-        <v>17</v>
-      </c>
       <c r="F35" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" t="s">
         <v>18</v>
       </c>
-      <c r="G35" t="s">
-        <v>19</v>
-      </c>
-      <c r="H35" s="14" t="s">
+      <c r="H35" t="s">
+        <v>19</v>
+      </c>
+      <c r="I35" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="I35" s="13" t="s">
+      <c r="J35" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <v>2008</v>
       </c>
-      <c r="K35">
+      <c r="L35">
         <v>26</v>
       </c>
-      <c r="L35" t="s">
+      <c r="M35" t="s">
         <v>86</v>
       </c>
-      <c r="M35" s="4">
+      <c r="N35" s="4">
         <v>18639552</v>
       </c>
-      <c r="N35" s="2" t="s">
+      <c r="O35" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>15</v>
       </c>
@@ -2792,35 +2883,35 @@
       <c r="C36" t="s">
         <v>16</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="E36" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="E36" t="s">
-        <v>17</v>
-      </c>
       <c r="F36" t="s">
+        <v>17</v>
+      </c>
+      <c r="G36" t="s">
         <v>18</v>
       </c>
-      <c r="G36" t="s">
-        <v>19</v>
-      </c>
-      <c r="H36" s="13" t="s">
+      <c r="H36" t="s">
+        <v>19</v>
+      </c>
+      <c r="I36" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="I36" s="13" t="s">
+      <c r="J36" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="J36">
+      <c r="K36">
         <v>2013</v>
       </c>
-      <c r="K36">
+      <c r="L36">
         <v>69</v>
       </c>
-      <c r="L36" t="s">
+      <c r="M36" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -2830,41 +2921,41 @@
       <c r="C37" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="E37" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="E37" t="s">
-        <v>17</v>
-      </c>
       <c r="F37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" t="s">
         <v>18</v>
       </c>
-      <c r="G37" t="s">
-        <v>19</v>
-      </c>
-      <c r="H37" s="13" t="s">
+      <c r="H37" t="s">
+        <v>19</v>
+      </c>
+      <c r="I37" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="I37" s="13" t="s">
+      <c r="J37" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J37">
+      <c r="K37">
         <v>2019</v>
       </c>
-      <c r="K37">
+      <c r="L37">
         <v>243</v>
       </c>
-      <c r="L37" t="s">
+      <c r="M37" t="s">
         <v>242</v>
       </c>
-      <c r="M37" s="4">
+      <c r="N37" s="4">
         <v>31679176</v>
       </c>
-      <c r="N37" s="2" t="s">
+      <c r="O37" s="2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>15</v>
       </c>
@@ -2874,38 +2965,41 @@
       <c r="C38" t="s">
         <v>16</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D38" t="s">
+        <v>262</v>
+      </c>
+      <c r="E38" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="E38" t="s">
-        <v>17</v>
-      </c>
       <c r="F38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G38" t="s">
         <v>18</v>
       </c>
-      <c r="G38" t="s">
-        <v>19</v>
-      </c>
-      <c r="H38" s="13" t="s">
+      <c r="H38" t="s">
+        <v>19</v>
+      </c>
+      <c r="I38" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="I38" s="13" t="s">
+      <c r="J38" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J38">
+      <c r="K38">
         <v>2019</v>
       </c>
-      <c r="K38">
+      <c r="L38">
         <v>242</v>
       </c>
-      <c r="M38" s="4">
+      <c r="N38" s="4">
         <v>30773443</v>
       </c>
-      <c r="N38" s="2" t="s">
+      <c r="O38" s="2" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>15</v>
       </c>
@@ -2915,41 +3009,44 @@
       <c r="C39" t="s">
         <v>16</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="D39" t="s">
+        <v>262</v>
+      </c>
+      <c r="E39" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="E39" t="s">
-        <v>17</v>
-      </c>
       <c r="F39" t="s">
+        <v>17</v>
+      </c>
+      <c r="G39" t="s">
         <v>18</v>
       </c>
-      <c r="G39" t="s">
-        <v>19</v>
-      </c>
-      <c r="H39" s="13" t="s">
+      <c r="H39" t="s">
+        <v>19</v>
+      </c>
+      <c r="I39" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="I39" s="13" t="s">
+      <c r="J39" s="13" t="s">
         <v>251</v>
       </c>
-      <c r="J39">
+      <c r="K39">
         <v>2004</v>
       </c>
-      <c r="K39">
+      <c r="L39">
         <v>34</v>
       </c>
-      <c r="L39" t="s">
+      <c r="M39" t="s">
         <v>252</v>
       </c>
-      <c r="M39" s="4">
+      <c r="N39" s="4">
         <v>12958056</v>
       </c>
-      <c r="N39" s="2" t="s">
+      <c r="O39" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -2959,41 +3056,41 @@
       <c r="C40" t="s">
         <v>16</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="E40" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="E40" t="s">
-        <v>17</v>
-      </c>
       <c r="F40" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" t="s">
         <v>18</v>
       </c>
-      <c r="G40" t="s">
-        <v>19</v>
-      </c>
-      <c r="H40" s="13" t="s">
+      <c r="H40" t="s">
+        <v>19</v>
+      </c>
+      <c r="I40" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="I40" s="13" t="s">
+      <c r="J40" s="13" t="s">
         <v>251</v>
       </c>
-      <c r="J40">
+      <c r="K40">
         <v>2008</v>
       </c>
-      <c r="K40">
+      <c r="L40">
         <v>32</v>
       </c>
-      <c r="L40" t="s">
+      <c r="M40" t="s">
         <v>256</v>
       </c>
-      <c r="M40" s="4">
+      <c r="N40" s="4">
         <v>18212627</v>
       </c>
-      <c r="N40" s="2" t="s">
+      <c r="O40" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>15</v>
       </c>
@@ -3003,41 +3100,44 @@
       <c r="C41" t="s">
         <v>16</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D41" t="s">
+        <v>262</v>
+      </c>
+      <c r="E41" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="E41" t="s">
-        <v>17</v>
-      </c>
       <c r="F41" t="s">
+        <v>17</v>
+      </c>
+      <c r="G41" t="s">
         <v>18</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>76</v>
       </c>
-      <c r="H41" s="13" t="s">
+      <c r="I41" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="I41" s="13" t="s">
+      <c r="J41" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="J41">
+      <c r="K41">
         <v>2020</v>
       </c>
-      <c r="K41">
+      <c r="L41">
         <v>48</v>
       </c>
-      <c r="L41" t="s">
+      <c r="M41" t="s">
         <v>20</v>
       </c>
-      <c r="M41" s="4">
+      <c r="N41" s="4">
         <v>33705361</v>
       </c>
-      <c r="N41" s="2" t="s">
+      <c r="O41" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -3047,38 +3147,41 @@
       <c r="C42" t="s">
         <v>16</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" t="s">
+        <v>265</v>
+      </c>
+      <c r="E42" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E42" t="s">
-        <v>17</v>
-      </c>
       <c r="F42" t="s">
+        <v>17</v>
+      </c>
+      <c r="G42" t="s">
         <v>114</v>
       </c>
-      <c r="G42" t="s">
-        <v>19</v>
-      </c>
-      <c r="H42" s="13" t="s">
+      <c r="H42" t="s">
+        <v>19</v>
+      </c>
+      <c r="I42" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="I42" s="13" t="s">
+      <c r="J42" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="J42">
+      <c r="K42">
         <v>2016</v>
       </c>
-      <c r="M42" s="4">
+      <c r="N42" s="4">
         <v>27452608</v>
       </c>
-      <c r="N42" s="2" t="s">
+      <c r="O42" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="O42" s="8" t="s">
+      <c r="P42" s="8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>15</v>
       </c>
@@ -3088,41 +3191,44 @@
       <c r="C43" t="s">
         <v>16</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" t="s">
+        <v>265</v>
+      </c>
+      <c r="E43" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E43" t="s">
-        <v>17</v>
-      </c>
       <c r="F43" t="s">
+        <v>17</v>
+      </c>
+      <c r="G43" t="s">
         <v>124</v>
       </c>
-      <c r="G43" t="s">
-        <v>19</v>
-      </c>
-      <c r="H43" s="14" t="s">
+      <c r="H43" t="s">
+        <v>19</v>
+      </c>
+      <c r="I43" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="I43" s="14" t="s">
+      <c r="J43" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="J43">
+      <c r="K43">
         <v>2009</v>
       </c>
-      <c r="K43">
+      <c r="L43">
         <v>82</v>
       </c>
-      <c r="L43" t="s">
+      <c r="M43" t="s">
         <v>127</v>
       </c>
-      <c r="M43" s="4">
+      <c r="N43" s="4">
         <v>19017305</v>
       </c>
-      <c r="N43" s="2" t="s">
+      <c r="O43" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>15</v>
       </c>
@@ -3132,41 +3238,41 @@
       <c r="C44" t="s">
         <v>47</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="E44" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E44" t="s">
-        <v>17</v>
-      </c>
       <c r="F44" t="s">
+        <v>17</v>
+      </c>
+      <c r="G44" t="s">
         <v>18</v>
       </c>
-      <c r="G44" t="s">
-        <v>19</v>
-      </c>
-      <c r="H44" s="13" t="s">
+      <c r="H44" t="s">
+        <v>19</v>
+      </c>
+      <c r="I44" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="I44" s="13" t="s">
+      <c r="J44" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="J44">
+      <c r="K44">
         <v>2004</v>
       </c>
-      <c r="K44">
+      <c r="L44">
         <v>21</v>
       </c>
-      <c r="L44" s="6" t="s">
+      <c r="M44" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="M44" s="4">
+      <c r="N44" s="4">
         <v>15583081</v>
       </c>
-      <c r="N44" s="2" t="s">
+      <c r="O44" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>15</v>
       </c>
@@ -3176,41 +3282,44 @@
       <c r="C45" t="s">
         <v>16</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" t="s">
+        <v>265</v>
+      </c>
+      <c r="E45" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E45" t="s">
-        <v>17</v>
-      </c>
       <c r="F45" t="s">
+        <v>17</v>
+      </c>
+      <c r="G45" t="s">
         <v>18</v>
       </c>
-      <c r="G45" t="s">
-        <v>19</v>
-      </c>
-      <c r="H45" s="14" t="s">
+      <c r="H45" t="s">
+        <v>19</v>
+      </c>
+      <c r="I45" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="I45" s="13" t="s">
+      <c r="J45" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J45">
+      <c r="K45">
         <v>2010</v>
       </c>
-      <c r="K45">
+      <c r="L45">
         <v>105</v>
       </c>
-      <c r="L45" t="s">
+      <c r="M45" t="s">
         <v>90</v>
       </c>
-      <c r="M45" s="4">
+      <c r="N45" s="4">
         <v>20501945</v>
       </c>
-      <c r="N45" s="2" t="s">
+      <c r="O45" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>15</v>
       </c>
@@ -3220,41 +3329,44 @@
       <c r="C46" t="s">
         <v>47</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D46" t="s">
+        <v>265</v>
+      </c>
+      <c r="E46" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E46" t="s">
-        <v>17</v>
-      </c>
       <c r="F46" t="s">
+        <v>17</v>
+      </c>
+      <c r="G46" t="s">
         <v>18</v>
       </c>
-      <c r="G46" t="s">
-        <v>19</v>
-      </c>
-      <c r="H46" s="13" t="s">
+      <c r="H46" t="s">
+        <v>19</v>
+      </c>
+      <c r="I46" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="I46" s="13" t="s">
+      <c r="J46" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="J46">
+      <c r="K46">
         <v>2012</v>
       </c>
-      <c r="K46">
+      <c r="L46">
         <v>102</v>
       </c>
-      <c r="L46" t="s">
+      <c r="M46" t="s">
         <v>186</v>
       </c>
-      <c r="M46" s="4">
+      <c r="N46" s="4">
         <v>23009139</v>
       </c>
-      <c r="N46" s="2" t="s">
+      <c r="O46" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>15</v>
       </c>
@@ -3264,41 +3376,44 @@
       <c r="C47" t="s">
         <v>16</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" t="s">
+        <v>265</v>
+      </c>
+      <c r="E47" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E47" t="s">
-        <v>17</v>
-      </c>
-      <c r="F47" s="2" t="s">
+      <c r="F47" t="s">
+        <v>17</v>
+      </c>
+      <c r="G47" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G47" t="s">
-        <v>19</v>
-      </c>
-      <c r="H47" s="13" t="s">
+      <c r="H47" t="s">
+        <v>19</v>
+      </c>
+      <c r="I47" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="I47" s="13" t="s">
+      <c r="J47" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J47">
+      <c r="K47">
         <v>2018</v>
       </c>
-      <c r="K47">
+      <c r="L47">
         <v>530</v>
       </c>
-      <c r="L47" t="s">
+      <c r="M47" t="s">
         <v>60</v>
       </c>
-      <c r="M47" s="4">
+      <c r="N47" s="4">
         <v>29985559</v>
       </c>
-      <c r="N47" s="2" t="s">
+      <c r="O47" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>15</v>
       </c>
@@ -3308,38 +3423,41 @@
       <c r="C48" t="s">
         <v>47</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" t="s">
+        <v>265</v>
+      </c>
+      <c r="E48" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E48" t="s">
-        <v>17</v>
-      </c>
       <c r="F48" t="s">
+        <v>17</v>
+      </c>
+      <c r="G48" t="s">
         <v>212</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>151</v>
       </c>
-      <c r="H48" s="13" t="s">
+      <c r="I48" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="I48" s="13" t="s">
+      <c r="J48" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="J48">
+      <c r="K48">
         <v>2019</v>
       </c>
-      <c r="K48">
+      <c r="L48">
         <v>153</v>
       </c>
-      <c r="M48" s="4">
+      <c r="N48" s="4">
         <v>31278196</v>
       </c>
-      <c r="N48" s="2" t="s">
+      <c r="O48" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>15</v>
       </c>
@@ -3349,41 +3467,44 @@
       <c r="C49" t="s">
         <v>16</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" t="s">
+        <v>265</v>
+      </c>
+      <c r="E49" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E49" t="s">
-        <v>17</v>
-      </c>
       <c r="F49" t="s">
+        <v>17</v>
+      </c>
+      <c r="G49" t="s">
         <v>94</v>
       </c>
-      <c r="G49" t="s">
-        <v>19</v>
-      </c>
-      <c r="H49" s="13" t="s">
+      <c r="H49" t="s">
+        <v>19</v>
+      </c>
+      <c r="I49" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="I49" s="13" t="s">
+      <c r="J49" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="J49">
+      <c r="K49">
         <v>2011</v>
       </c>
-      <c r="K49">
+      <c r="L49">
         <v>120</v>
       </c>
-      <c r="L49" t="s">
+      <c r="M49" t="s">
         <v>96</v>
       </c>
-      <c r="M49" s="4">
+      <c r="N49" s="4">
         <v>21881554</v>
       </c>
-      <c r="N49" s="2" t="s">
+      <c r="O49" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>15</v>
       </c>
@@ -3393,38 +3514,41 @@
       <c r="C50" t="s">
         <v>16</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" t="s">
+        <v>265</v>
+      </c>
+      <c r="E50" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E50" t="s">
-        <v>17</v>
-      </c>
       <c r="F50" t="s">
+        <v>17</v>
+      </c>
+      <c r="G50" t="s">
         <v>94</v>
       </c>
-      <c r="G50" t="s">
-        <v>19</v>
-      </c>
-      <c r="H50" s="15" t="s">
+      <c r="H50" t="s">
+        <v>19</v>
+      </c>
+      <c r="I50" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="I50" s="13" t="s">
+      <c r="J50" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J50">
+      <c r="K50">
         <v>2013</v>
       </c>
-      <c r="K50">
+      <c r="L50">
         <v>306</v>
       </c>
-      <c r="M50" s="4">
+      <c r="N50" s="4">
         <v>23915426</v>
       </c>
-      <c r="N50" s="2" t="s">
+      <c r="O50" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -3434,41 +3558,44 @@
       <c r="C51" t="s">
         <v>16</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" t="s">
+        <v>266</v>
+      </c>
+      <c r="E51" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E51" t="s">
-        <v>17</v>
-      </c>
       <c r="F51" t="s">
+        <v>17</v>
+      </c>
+      <c r="G51" t="s">
         <v>94</v>
       </c>
-      <c r="G51" t="s">
-        <v>19</v>
-      </c>
-      <c r="H51" s="13" t="s">
+      <c r="H51" t="s">
+        <v>19</v>
+      </c>
+      <c r="I51" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="I51" s="13" t="s">
+      <c r="J51" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="J51">
+      <c r="K51">
         <v>2015</v>
       </c>
-      <c r="K51">
+      <c r="L51">
         <v>76</v>
       </c>
-      <c r="L51" t="s">
+      <c r="M51" t="s">
         <v>144</v>
       </c>
-      <c r="M51" s="4">
+      <c r="N51" s="4">
         <v>27369853</v>
       </c>
-      <c r="N51" s="2" t="s">
+      <c r="O51" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>15</v>
       </c>
@@ -3478,41 +3605,44 @@
       <c r="C52" t="s">
         <v>16</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D52" t="s">
+        <v>266</v>
+      </c>
+      <c r="E52" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E52" t="s">
-        <v>17</v>
-      </c>
       <c r="F52" t="s">
+        <v>17</v>
+      </c>
+      <c r="G52" t="s">
         <v>94</v>
       </c>
-      <c r="G52" t="s">
+      <c r="H52" t="s">
         <v>151</v>
       </c>
-      <c r="H52" s="13" t="s">
+      <c r="I52" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="I52" s="13" t="s">
+      <c r="J52" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="J52">
+      <c r="K52">
         <v>2019</v>
       </c>
-      <c r="K52">
+      <c r="L52">
         <v>34</v>
       </c>
-      <c r="L52" t="s">
+      <c r="M52" t="s">
         <v>159</v>
       </c>
-      <c r="M52" s="4">
+      <c r="N52" s="4">
         <v>31292297</v>
       </c>
-      <c r="N52" s="2" t="s">
+      <c r="O52" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>15</v>
       </c>
@@ -3522,41 +3652,41 @@
       <c r="C53" t="s">
         <v>16</v>
       </c>
-      <c r="D53" s="10" t="s">
+      <c r="E53" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="E53" t="s">
-        <v>17</v>
-      </c>
       <c r="F53" t="s">
+        <v>17</v>
+      </c>
+      <c r="G53" t="s">
         <v>94</v>
       </c>
-      <c r="G53" t="s">
-        <v>19</v>
-      </c>
-      <c r="H53" s="13" t="s">
+      <c r="H53" t="s">
+        <v>19</v>
+      </c>
+      <c r="I53" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="I53" s="13" t="s">
+      <c r="J53" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J53">
+      <c r="K53">
         <v>2020</v>
       </c>
-      <c r="K53">
+      <c r="L53">
         <v>235</v>
       </c>
-      <c r="L53" t="s">
+      <c r="M53" t="s">
         <v>232</v>
       </c>
-      <c r="M53" s="4">
+      <c r="N53" s="4">
         <v>32090446</v>
       </c>
-      <c r="N53" s="2" t="s">
+      <c r="O53" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -3566,41 +3696,44 @@
       <c r="C54" t="s">
         <v>16</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D54" t="s">
+        <v>266</v>
+      </c>
+      <c r="E54" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E54" t="s">
-        <v>17</v>
-      </c>
       <c r="F54" t="s">
+        <v>17</v>
+      </c>
+      <c r="G54" t="s">
         <v>106</v>
       </c>
-      <c r="G54" t="s">
-        <v>19</v>
-      </c>
-      <c r="H54" s="13" t="s">
+      <c r="H54" t="s">
+        <v>19</v>
+      </c>
+      <c r="I54" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="I54" s="13" t="s">
+      <c r="J54" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J54">
+      <c r="K54">
         <v>2014</v>
       </c>
-      <c r="K54">
+      <c r="L54">
         <v>411</v>
       </c>
-      <c r="L54" t="s">
+      <c r="M54" t="s">
         <v>108</v>
       </c>
-      <c r="M54" s="4">
+      <c r="N54" s="4">
         <v>25377077</v>
       </c>
-      <c r="N54" s="2" t="s">
+      <c r="O54" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>15</v>
       </c>
@@ -3610,41 +3743,44 @@
       <c r="C55" t="s">
         <v>16</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D55" t="s">
+        <v>266</v>
+      </c>
+      <c r="E55" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E55" t="s">
-        <v>17</v>
-      </c>
       <c r="F55" t="s">
+        <v>17</v>
+      </c>
+      <c r="G55" t="s">
         <v>106</v>
       </c>
-      <c r="G55" t="s">
+      <c r="H55" t="s">
         <v>151</v>
       </c>
-      <c r="H55" s="13" t="s">
+      <c r="I55" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="I55" s="13" t="s">
+      <c r="J55" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="J55">
+      <c r="K55">
         <v>2018</v>
       </c>
-      <c r="K55">
-        <v>16</v>
-      </c>
-      <c r="L55" t="s">
+      <c r="L55">
+        <v>16</v>
+      </c>
+      <c r="M55" t="s">
         <v>154</v>
       </c>
-      <c r="M55" s="4">
+      <c r="N55" s="4">
         <v>30341925</v>
       </c>
-      <c r="N55" s="2" t="s">
+      <c r="O55" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>15</v>
       </c>
@@ -3654,41 +3790,44 @@
       <c r="C56" t="s">
         <v>16</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D56" t="s">
+        <v>266</v>
+      </c>
+      <c r="E56" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E56" t="s">
-        <v>17</v>
-      </c>
       <c r="F56" t="s">
+        <v>17</v>
+      </c>
+      <c r="G56" t="s">
         <v>106</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>151</v>
       </c>
-      <c r="H56" s="13" t="s">
+      <c r="I56" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="I56" s="13" t="s">
+      <c r="J56" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="J56">
+      <c r="K56">
         <v>2019</v>
       </c>
-      <c r="K56">
+      <c r="L56">
         <v>30</v>
       </c>
-      <c r="L56" t="s">
+      <c r="M56" t="s">
         <v>164</v>
       </c>
-      <c r="M56" s="4">
+      <c r="N56" s="4">
         <v>31208411</v>
       </c>
-      <c r="N56" s="2" t="s">
+      <c r="O56" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>15</v>
       </c>
@@ -3698,41 +3837,41 @@
       <c r="C57" t="s">
         <v>16</v>
       </c>
-      <c r="D57" s="11" t="s">
+      <c r="E57" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="E57" t="s">
-        <v>17</v>
-      </c>
       <c r="F57" t="s">
+        <v>17</v>
+      </c>
+      <c r="G57" t="s">
         <v>106</v>
       </c>
-      <c r="G57" t="s">
-        <v>19</v>
-      </c>
-      <c r="H57" s="13" t="s">
+      <c r="H57" t="s">
+        <v>19</v>
+      </c>
+      <c r="I57" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="I57" s="13" t="s">
+      <c r="J57" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J57">
+      <c r="K57">
         <v>2020</v>
       </c>
-      <c r="K57">
+      <c r="L57">
         <v>771</v>
       </c>
-      <c r="L57" t="s">
+      <c r="M57" t="s">
         <v>247</v>
       </c>
-      <c r="M57" s="4">
+      <c r="N57" s="4">
         <v>32943286</v>
       </c>
-      <c r="N57" s="2" t="s">
+      <c r="O57" s="2" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>15</v>
       </c>
@@ -3742,41 +3881,44 @@
       <c r="C58" t="s">
         <v>16</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="D58" t="s">
+        <v>266</v>
+      </c>
+      <c r="E58" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E58" t="s">
-        <v>17</v>
-      </c>
       <c r="F58" t="s">
+        <v>17</v>
+      </c>
+      <c r="G58" t="s">
         <v>130</v>
       </c>
-      <c r="G58" t="s">
-        <v>19</v>
-      </c>
-      <c r="H58" s="13" t="s">
+      <c r="H58" t="s">
+        <v>19</v>
+      </c>
+      <c r="I58" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="I58" s="13" t="s">
+      <c r="J58" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J58">
+      <c r="K58">
         <v>2017</v>
       </c>
-      <c r="K58">
+      <c r="L58">
         <v>1208</v>
       </c>
-      <c r="L58" t="s">
+      <c r="M58" t="s">
         <v>132</v>
       </c>
-      <c r="M58" s="4">
+      <c r="N58" s="4">
         <v>28614805</v>
       </c>
-      <c r="N58" s="2" t="s">
+      <c r="O58" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>15</v>
       </c>
@@ -3786,99 +3928,109 @@
       <c r="C59" t="s">
         <v>16</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="D59" t="s">
+        <v>266</v>
+      </c>
+      <c r="E59" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E59" t="s">
-        <v>17</v>
-      </c>
       <c r="F59" t="s">
+        <v>17</v>
+      </c>
+      <c r="G59" t="s">
         <v>120</v>
       </c>
-      <c r="G59" t="s">
-        <v>19</v>
-      </c>
-      <c r="H59" s="13" t="s">
+      <c r="H59" t="s">
+        <v>19</v>
+      </c>
+      <c r="I59" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="I59" s="13" t="s">
+      <c r="J59" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="J59">
+      <c r="K59">
         <v>2016</v>
       </c>
-      <c r="K59">
+      <c r="L59">
         <v>153</v>
       </c>
-      <c r="L59" t="s">
+      <c r="M59" t="s">
         <v>121</v>
       </c>
-      <c r="M59" s="4">
+      <c r="N59" s="4">
         <v>26990570</v>
       </c>
-      <c r="N59" s="2" t="s">
+      <c r="O59" s="2" t="s">
         <v>122</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O89">
-    <sortCondition ref="F1:F89"/>
+  <autoFilter ref="A1:P59" xr:uid="{62D030C5-8C54-2A48-90BC-6F06473898BD}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Kidney"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P89">
+    <sortCondition ref="G1:G89"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="M44" r:id="rId1" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/15583081" xr:uid="{785BC3EA-DA10-AC43-819B-AF8461511ABD}"/>
-    <hyperlink ref="M4" r:id="rId2" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/31378695" xr:uid="{4F2B4DDA-6B1D-8C4A-8C49-2A0EABD2D17C}"/>
-    <hyperlink ref="M2" r:id="rId3" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/31378695" xr:uid="{6C8D648B-8361-BA46-9242-71CD3A8AD325}"/>
-    <hyperlink ref="M58" r:id="rId4" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/28614805" xr:uid="{8AC3EBA4-EEB5-D244-B951-B5FBDC988D9A}"/>
-    <hyperlink ref="M6" r:id="rId5" display="http://europepmc.org/abstract/MED/27898719" xr:uid="{569A20A3-A9B2-704A-9805-66B0D2D42139}"/>
-    <hyperlink ref="M7" r:id="rId6" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/16433769" xr:uid="{B0A0C97F-D062-4D44-9040-C2DD048273C1}"/>
-    <hyperlink ref="M46" r:id="rId7" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/23009139" xr:uid="{5C0051B8-1E7F-2B44-BD67-A322063CEAE6}"/>
-    <hyperlink ref="M9" r:id="rId8" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/24725967" xr:uid="{EA074AF7-3D61-DD41-BE6E-B1E910580A52}"/>
-    <hyperlink ref="M45" r:id="rId9" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/20501945" xr:uid="{03358325-AD19-8D45-9CD2-E6A61065C1EB}"/>
-    <hyperlink ref="M10" r:id="rId10" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/25387159" xr:uid="{D88CA2DE-FAE8-1948-AAA7-19677227A737}"/>
-    <hyperlink ref="M59" r:id="rId11" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/26990570" xr:uid="{847CD4BF-2292-F84D-AA97-91C976F43FBB}"/>
-    <hyperlink ref="M13" r:id="rId12" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/26484130" xr:uid="{BC9618FF-0D4F-E24B-93A7-7E7C15E675ED}"/>
-    <hyperlink ref="M47" r:id="rId13" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/29985559" xr:uid="{D2B5242C-FA36-9540-AC82-FB7820F9B33F}"/>
-    <hyperlink ref="M28" r:id="rId14" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/31167967" xr:uid="{24C3B031-A544-C24D-A1E6-BFDFCBA8DD59}"/>
-    <hyperlink ref="M16" r:id="rId15" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/16780603" xr:uid="{B2FC032F-4639-1F4A-AB3E-ED072187AF9D}"/>
-    <hyperlink ref="M31" r:id="rId16" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/20208531" xr:uid="{C8F57D5A-AD61-8448-82F6-41CAD81D36D6}"/>
-    <hyperlink ref="M12" r:id="rId17" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/26517400" xr:uid="{FD4180AF-C6C0-2043-BA61-8CC1C9D1A196}"/>
-    <hyperlink ref="M17" r:id="rId18" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/16794196" xr:uid="{5F71B3B6-8FEB-9049-B23D-89ED4B44D9FC}"/>
-    <hyperlink ref="M20" r:id="rId19" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/20150539" xr:uid="{DE2D30FE-2D8B-3449-8456-154EF5988532}"/>
-    <hyperlink ref="M15" r:id="rId20" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/16794196" xr:uid="{67B5D7E6-DF59-EA45-BDBE-B769A8AC98EE}"/>
-    <hyperlink ref="M18" r:id="rId21" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/21555702" xr:uid="{C3C6CA03-D213-1848-876E-DAC0465E846E}"/>
-    <hyperlink ref="M38" r:id="rId22" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/30773443" xr:uid="{35F0DCDB-D3CC-A14E-8DAC-8C0F91C9B3A9}"/>
-    <hyperlink ref="M32" r:id="rId23" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/21827613" xr:uid="{540C7EB8-B1B7-B14F-BFC8-B574E835C818}"/>
-    <hyperlink ref="M34" r:id="rId24" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/18639552" xr:uid="{E19477A1-6265-1243-BC8B-ADFD0B7F8A47}"/>
-    <hyperlink ref="M35" r:id="rId25" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/18639552" xr:uid="{7E3910A3-9B40-F74E-B321-7F6FB8E053CA}"/>
-    <hyperlink ref="M37" r:id="rId26" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/31679176" xr:uid="{C84556D9-70B9-224D-9A43-02E8DF879323}"/>
-    <hyperlink ref="M11" r:id="rId27" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/19938108" xr:uid="{DF2199E4-E345-3A4A-B3F7-8721C77DB208}"/>
-    <hyperlink ref="M21" r:id="rId28" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/32669324" xr:uid="{D135C73C-AA77-E540-B2D8-87392A6F33AF}"/>
-    <hyperlink ref="M29" r:id="rId29" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/32669324" xr:uid="{B8466DD6-B301-0C4A-996F-2458CA65654F}"/>
-    <hyperlink ref="M30" r:id="rId30" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/15307835" xr:uid="{1FDC2779-D8C6-A343-AB00-BFD1043D01D8}"/>
-    <hyperlink ref="M22" r:id="rId31" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/15307835" xr:uid="{481E0A1B-DAD1-AF4D-AD51-0DF1BF19EAD2}"/>
-    <hyperlink ref="M23" r:id="rId32" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/21130165" xr:uid="{8554D442-A328-0E4D-BF8C-84039F7335B1}"/>
-    <hyperlink ref="M25" r:id="rId33" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/23437201" xr:uid="{04A46C98-C6FD-4149-B86B-E44AE6A68AD8}"/>
-    <hyperlink ref="M54" r:id="rId34" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/25377077" xr:uid="{509D8BDD-1B2D-6640-88AB-3F5EA929AECA}"/>
-    <hyperlink ref="M50" r:id="rId35" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/23915426" xr:uid="{1A6EB7BD-97BB-C74C-BF8B-EAF084DC0E53}"/>
-    <hyperlink ref="M5" r:id="rId36" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/25925804" xr:uid="{5AE1351C-9F51-D848-83C1-150F61C37345}"/>
-    <hyperlink ref="M42" r:id="rId37" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/27452608" xr:uid="{E8E2DE5D-2BCD-BE4C-A4D9-A06F1070BE6F}"/>
-    <hyperlink ref="M43" r:id="rId38" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/19017305" xr:uid="{9C70865A-5C3F-B945-8B44-CB19AD6B34F8}"/>
-    <hyperlink ref="M49" r:id="rId39" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/21881554" xr:uid="{420D4CB3-EFCB-EA45-8EBC-9075493EE800}"/>
-    <hyperlink ref="M8" r:id="rId40" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/12853585" xr:uid="{C493A428-96A4-C140-A103-1C51CF4A7C40}"/>
-    <hyperlink ref="M53" r:id="rId41" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/32090446" xr:uid="{896E4A51-655B-C844-BE9C-A7C0F4D1C159}"/>
-    <hyperlink ref="M3" r:id="rId42" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/22335458" xr:uid="{C5269F46-F7A1-EB4C-8AB6-511EBE82F69D}"/>
-    <hyperlink ref="M14" r:id="rId43" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/24698514" xr:uid="{4CD62B5C-76C0-8645-A15B-8B18709482D7}"/>
-    <hyperlink ref="M51" r:id="rId44" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/27369853" xr:uid="{AD506628-48FA-5242-BF9E-6BBB8D476391}"/>
-    <hyperlink ref="M26" r:id="rId45" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/27165815" xr:uid="{47E03DA9-E7EE-8144-8F84-517D6BC08D5B}"/>
-    <hyperlink ref="M57" r:id="rId46" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/32943286" xr:uid="{0112CF56-9B72-E748-BA99-FCF67B977DC4}"/>
-    <hyperlink ref="M39" r:id="rId47" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/12958056" xr:uid="{2BDBA9B1-176E-7F48-A3AB-C22747731B3E}"/>
-    <hyperlink ref="M40" r:id="rId48" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/18212627" xr:uid="{040BB413-9B38-9642-9B83-097908D740BB}"/>
-    <hyperlink ref="M41" r:id="rId49" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/33705361" xr:uid="{B6821AB6-66B8-6642-9533-6DB7BB4181DA}"/>
-    <hyperlink ref="M55" r:id="rId50" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/30341925" xr:uid="{EE7BD2FC-D5CA-AA4F-AE61-DC75EE99B3A6}"/>
-    <hyperlink ref="M48" r:id="rId51" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/31278196" xr:uid="{3A761127-942B-0844-9E8C-7FB33825B0CB}"/>
-    <hyperlink ref="M52" r:id="rId52" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/31292297" xr:uid="{E3C1FD48-DA1A-A04C-A4CB-B8ADC1C2D4E0}"/>
-    <hyperlink ref="M56" r:id="rId53" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/31208411" xr:uid="{0729E1D1-ACEB-434F-8200-A65111681998}"/>
-    <hyperlink ref="M27" r:id="rId54" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/29980650" xr:uid="{553B7191-E748-0C48-A951-57E072D3899D}"/>
+    <hyperlink ref="N44" r:id="rId1" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/15583081" xr:uid="{785BC3EA-DA10-AC43-819B-AF8461511ABD}"/>
+    <hyperlink ref="N4" r:id="rId2" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/31378695" xr:uid="{4F2B4DDA-6B1D-8C4A-8C49-2A0EABD2D17C}"/>
+    <hyperlink ref="N2" r:id="rId3" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/31378695" xr:uid="{6C8D648B-8361-BA46-9242-71CD3A8AD325}"/>
+    <hyperlink ref="N58" r:id="rId4" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/28614805" xr:uid="{8AC3EBA4-EEB5-D244-B951-B5FBDC988D9A}"/>
+    <hyperlink ref="N6" r:id="rId5" display="http://europepmc.org/abstract/MED/27898719" xr:uid="{569A20A3-A9B2-704A-9805-66B0D2D42139}"/>
+    <hyperlink ref="N7" r:id="rId6" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/16433769" xr:uid="{B0A0C97F-D062-4D44-9040-C2DD048273C1}"/>
+    <hyperlink ref="N46" r:id="rId7" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/23009139" xr:uid="{5C0051B8-1E7F-2B44-BD67-A322063CEAE6}"/>
+    <hyperlink ref="N9" r:id="rId8" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/24725967" xr:uid="{EA074AF7-3D61-DD41-BE6E-B1E910580A52}"/>
+    <hyperlink ref="N45" r:id="rId9" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/20501945" xr:uid="{03358325-AD19-8D45-9CD2-E6A61065C1EB}"/>
+    <hyperlink ref="N10" r:id="rId10" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/25387159" xr:uid="{D88CA2DE-FAE8-1948-AAA7-19677227A737}"/>
+    <hyperlink ref="N59" r:id="rId11" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/26990570" xr:uid="{847CD4BF-2292-F84D-AA97-91C976F43FBB}"/>
+    <hyperlink ref="N13" r:id="rId12" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/26484130" xr:uid="{BC9618FF-0D4F-E24B-93A7-7E7C15E675ED}"/>
+    <hyperlink ref="N47" r:id="rId13" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/29985559" xr:uid="{D2B5242C-FA36-9540-AC82-FB7820F9B33F}"/>
+    <hyperlink ref="N28" r:id="rId14" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/31167967" xr:uid="{24C3B031-A544-C24D-A1E6-BFDFCBA8DD59}"/>
+    <hyperlink ref="N16" r:id="rId15" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/16780603" xr:uid="{B2FC032F-4639-1F4A-AB3E-ED072187AF9D}"/>
+    <hyperlink ref="N31" r:id="rId16" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/20208531" xr:uid="{C8F57D5A-AD61-8448-82F6-41CAD81D36D6}"/>
+    <hyperlink ref="N12" r:id="rId17" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/26517400" xr:uid="{FD4180AF-C6C0-2043-BA61-8CC1C9D1A196}"/>
+    <hyperlink ref="N17" r:id="rId18" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/16794196" xr:uid="{5F71B3B6-8FEB-9049-B23D-89ED4B44D9FC}"/>
+    <hyperlink ref="N20" r:id="rId19" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/20150539" xr:uid="{DE2D30FE-2D8B-3449-8456-154EF5988532}"/>
+    <hyperlink ref="N15" r:id="rId20" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/16794196" xr:uid="{67B5D7E6-DF59-EA45-BDBE-B769A8AC98EE}"/>
+    <hyperlink ref="N18" r:id="rId21" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/21555702" xr:uid="{C3C6CA03-D213-1848-876E-DAC0465E846E}"/>
+    <hyperlink ref="N38" r:id="rId22" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/30773443" xr:uid="{35F0DCDB-D3CC-A14E-8DAC-8C0F91C9B3A9}"/>
+    <hyperlink ref="N32" r:id="rId23" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/21827613" xr:uid="{540C7EB8-B1B7-B14F-BFC8-B574E835C818}"/>
+    <hyperlink ref="N34" r:id="rId24" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/18639552" xr:uid="{E19477A1-6265-1243-BC8B-ADFD0B7F8A47}"/>
+    <hyperlink ref="N35" r:id="rId25" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/18639552" xr:uid="{7E3910A3-9B40-F74E-B321-7F6FB8E053CA}"/>
+    <hyperlink ref="N37" r:id="rId26" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/31679176" xr:uid="{C84556D9-70B9-224D-9A43-02E8DF879323}"/>
+    <hyperlink ref="N11" r:id="rId27" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/19938108" xr:uid="{DF2199E4-E345-3A4A-B3F7-8721C77DB208}"/>
+    <hyperlink ref="N21" r:id="rId28" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/32669324" xr:uid="{D135C73C-AA77-E540-B2D8-87392A6F33AF}"/>
+    <hyperlink ref="N29" r:id="rId29" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/32669324" xr:uid="{B8466DD6-B301-0C4A-996F-2458CA65654F}"/>
+    <hyperlink ref="N30" r:id="rId30" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/15307835" xr:uid="{1FDC2779-D8C6-A343-AB00-BFD1043D01D8}"/>
+    <hyperlink ref="N22" r:id="rId31" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/15307835" xr:uid="{481E0A1B-DAD1-AF4D-AD51-0DF1BF19EAD2}"/>
+    <hyperlink ref="N23" r:id="rId32" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/21130165" xr:uid="{8554D442-A328-0E4D-BF8C-84039F7335B1}"/>
+    <hyperlink ref="N25" r:id="rId33" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/23437201" xr:uid="{04A46C98-C6FD-4149-B86B-E44AE6A68AD8}"/>
+    <hyperlink ref="N54" r:id="rId34" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/25377077" xr:uid="{509D8BDD-1B2D-6640-88AB-3F5EA929AECA}"/>
+    <hyperlink ref="N50" r:id="rId35" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/23915426" xr:uid="{1A6EB7BD-97BB-C74C-BF8B-EAF084DC0E53}"/>
+    <hyperlink ref="N5" r:id="rId36" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/25925804" xr:uid="{5AE1351C-9F51-D848-83C1-150F61C37345}"/>
+    <hyperlink ref="N42" r:id="rId37" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/27452608" xr:uid="{E8E2DE5D-2BCD-BE4C-A4D9-A06F1070BE6F}"/>
+    <hyperlink ref="N43" r:id="rId38" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/19017305" xr:uid="{9C70865A-5C3F-B945-8B44-CB19AD6B34F8}"/>
+    <hyperlink ref="N49" r:id="rId39" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/21881554" xr:uid="{420D4CB3-EFCB-EA45-8EBC-9075493EE800}"/>
+    <hyperlink ref="N8" r:id="rId40" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/12853585" xr:uid="{C493A428-96A4-C140-A103-1C51CF4A7C40}"/>
+    <hyperlink ref="N53" r:id="rId41" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/32090446" xr:uid="{896E4A51-655B-C844-BE9C-A7C0F4D1C159}"/>
+    <hyperlink ref="N3" r:id="rId42" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/22335458" xr:uid="{C5269F46-F7A1-EB4C-8AB6-511EBE82F69D}"/>
+    <hyperlink ref="N14" r:id="rId43" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/24698514" xr:uid="{4CD62B5C-76C0-8645-A15B-8B18709482D7}"/>
+    <hyperlink ref="N51" r:id="rId44" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/27369853" xr:uid="{AD506628-48FA-5242-BF9E-6BBB8D476391}"/>
+    <hyperlink ref="N26" r:id="rId45" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/27165815" xr:uid="{47E03DA9-E7EE-8144-8F84-517D6BC08D5B}"/>
+    <hyperlink ref="N57" r:id="rId46" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/32943286" xr:uid="{0112CF56-9B72-E748-BA99-FCF67B977DC4}"/>
+    <hyperlink ref="N39" r:id="rId47" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/12958056" xr:uid="{2BDBA9B1-176E-7F48-A3AB-C22747731B3E}"/>
+    <hyperlink ref="N40" r:id="rId48" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/18212627" xr:uid="{040BB413-9B38-9642-9B83-097908D740BB}"/>
+    <hyperlink ref="N41" r:id="rId49" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/33705361" xr:uid="{B6821AB6-66B8-6642-9533-6DB7BB4181DA}"/>
+    <hyperlink ref="N55" r:id="rId50" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/30341925" xr:uid="{EE7BD2FC-D5CA-AA4F-AE61-DC75EE99B3A6}"/>
+    <hyperlink ref="N48" r:id="rId51" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/31278196" xr:uid="{3A761127-942B-0844-9E8C-7FB33825B0CB}"/>
+    <hyperlink ref="N52" r:id="rId52" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/31292297" xr:uid="{E3C1FD48-DA1A-A04C-A4CB-B8ADC1C2D4E0}"/>
+    <hyperlink ref="N56" r:id="rId53" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/31208411" xr:uid="{0729E1D1-ACEB-434F-8200-A65111681998}"/>
+    <hyperlink ref="N27" r:id="rId54" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/29980650" xr:uid="{553B7191-E748-0C48-A951-57E072D3899D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>